<commit_message>
feat: Adicionado sistema CRUD com API REST e interface interativa
- API REST com FastAPI
- Interface interativa PowerShell
- Suporte a JSON
- Exportação Excel
- Documentação atualizada
</commit_message>
<xml_diff>
--- a/02_searches/data/screening_database.xlsx
+++ b/02_searches/data/screening_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0caab5ec85f65fc/Desktop/meta-analysis_neurocisticercosis/02_searches/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_23F921ED85E30AA48B93FDF735EB93E3550B5836" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BED88B45-6421-4CE0-B0AA-8F376A1CFCCB}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_23F921ED85E30AA48B93FDF735EB93E3550B5836" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F70A1B9-40FE-41CC-9298-FCFED1A8C432}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2471,12 +2471,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2508,12 +2514,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2896,8 +2903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="M90" sqref="M90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6640,708 +6647,787 @@
         <v>802</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A97">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A97" s="3">
         <v>26984901</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F97" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="G97">
+      <c r="G97" s="3">
         <v>2016</v>
       </c>
-      <c r="H97" t="s">
+      <c r="H97" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I97" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="K97" t="s">
+      <c r="J97" s="3"/>
+      <c r="K97" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="L97" t="s">
+      <c r="L97" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O97" t="s">
+      <c r="M97" s="3"/>
+      <c r="N97" s="3"/>
+      <c r="O97" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q97">
+      <c r="P97" s="3"/>
+      <c r="Q97" s="3">
         <v>2016</v>
       </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A98">
+      <c r="R97" s="3"/>
+      <c r="S97" s="3"/>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A98" s="3">
         <v>24999157</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F98" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="G98">
+      <c r="G98" s="3">
         <v>2014</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H98" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="I98" t="s">
+      <c r="I98" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="J98" t="s">
+      <c r="J98" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="K98" t="s">
+      <c r="K98" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="L98" t="s">
+      <c r="L98" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O98" t="s">
+      <c r="M98" s="3"/>
+      <c r="N98" s="3"/>
+      <c r="O98" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q98">
+      <c r="P98" s="3"/>
+      <c r="Q98" s="3">
         <v>2014</v>
       </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A99">
+      <c r="R98" s="3"/>
+      <c r="S98" s="3"/>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A99" s="3">
         <v>29579308</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F99" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="G99">
+      <c r="G99" s="3">
         <v>2018</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H99" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I99" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="K99" t="s">
+      <c r="J99" s="3"/>
+      <c r="K99" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="L99" t="s">
+      <c r="L99" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O99" t="s">
+      <c r="M99" s="3"/>
+      <c r="N99" s="3"/>
+      <c r="O99" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q99">
+      <c r="P99" s="3"/>
+      <c r="Q99" s="3">
         <v>2018</v>
       </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A100">
+      <c r="R99" s="3"/>
+      <c r="S99" s="3"/>
+    </row>
+    <row r="100" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="3">
         <v>25092547</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F100" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="G100">
+      <c r="G100" s="3">
         <v>2014</v>
       </c>
-      <c r="H100" t="s">
+      <c r="H100" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="I100" t="s">
+      <c r="I100" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="J100" t="s">
+      <c r="J100" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="K100" t="s">
+      <c r="K100" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="L100" t="s">
+      <c r="L100" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O100" t="s">
+      <c r="O100" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q100">
+      <c r="Q100" s="3">
         <v>2014</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A101">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A101" s="3">
         <v>26433183</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F101" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="G101">
+      <c r="G101" s="3">
         <v>2015</v>
       </c>
-      <c r="H101" t="s">
+      <c r="H101" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="K101" t="s">
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="L101" t="s">
+      <c r="L101" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O101" t="s">
+      <c r="M101" s="3"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q101">
+      <c r="P101" s="3"/>
+      <c r="Q101" s="3">
         <v>2015</v>
       </c>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A102">
+      <c r="R101" s="3"/>
+      <c r="S101" s="3"/>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A102" s="3">
         <v>33006755</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="G102">
+      <c r="G102" s="3">
         <v>2021</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H102" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="K102" t="s">
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3" t="s">
         <v>564</v>
       </c>
-      <c r="L102" t="s">
+      <c r="L102" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O102" t="s">
+      <c r="M102" s="3"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q102">
+      <c r="P102" s="3"/>
+      <c r="Q102" s="3">
         <v>2021</v>
       </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A103">
+      <c r="R102" s="3"/>
+      <c r="S102" s="3"/>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A103" s="3">
         <v>31355931</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E103" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="G103">
+      <c r="G103" s="3">
         <v>2019</v>
       </c>
-      <c r="H103" t="s">
+      <c r="H103" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="I103" t="s">
+      <c r="I103" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="J103" t="s">
+      <c r="J103" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="K103" t="s">
+      <c r="K103" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="L103" t="s">
+      <c r="L103" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O103" t="s">
+      <c r="M103" s="3"/>
+      <c r="N103" s="3"/>
+      <c r="O103" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q103">
+      <c r="P103" s="3"/>
+      <c r="Q103" s="3">
         <v>2019</v>
       </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A104">
+      <c r="R103" s="3"/>
+      <c r="S103" s="3"/>
+    </row>
+    <row r="104" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="3">
         <v>18495737</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F104" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="G104">
+      <c r="G104" s="3">
         <v>2008</v>
       </c>
-      <c r="H104" t="s">
+      <c r="H104" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="K104" t="s">
+      <c r="K104" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="L104" t="s">
+      <c r="L104" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O104" t="s">
+      <c r="O104" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q104">
+      <c r="Q104" s="3">
         <v>2008</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A105">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A105" s="3">
         <v>17964789</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="F105" t="s">
+      <c r="F105" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="G105">
+      <c r="G105" s="3">
         <v>2007</v>
       </c>
-      <c r="H105" t="s">
+      <c r="H105" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="K105" t="s">
+      <c r="I105" s="3"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="L105" t="s">
+      <c r="L105" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O105" t="s">
+      <c r="M105" s="3"/>
+      <c r="N105" s="3"/>
+      <c r="O105" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q105">
+      <c r="P105" s="3"/>
+      <c r="Q105" s="3">
         <v>2007</v>
       </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A106">
+      <c r="R105" s="3"/>
+      <c r="S105" s="3"/>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A106" s="3">
         <v>14724304</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E106" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F106" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="G106">
+      <c r="G106" s="3">
         <v>2004</v>
       </c>
-      <c r="H106" t="s">
+      <c r="H106" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="K106" t="s">
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="L106" t="s">
+      <c r="L106" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O106" t="s">
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q106">
+      <c r="P106" s="3"/>
+      <c r="Q106" s="3">
         <v>2004</v>
       </c>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A107">
+      <c r="R106" s="3"/>
+      <c r="S106" s="3"/>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A107" s="3">
         <v>17928325</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F107" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="G107">
+      <c r="G107" s="3">
         <v>2008</v>
       </c>
-      <c r="H107" t="s">
+      <c r="H107" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="K107" t="s">
+      <c r="I107" s="3"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="L107" t="s">
+      <c r="L107" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O107" t="s">
+      <c r="M107" s="3"/>
+      <c r="N107" s="3"/>
+      <c r="O107" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q107">
+      <c r="P107" s="3"/>
+      <c r="Q107" s="3">
         <v>2008</v>
       </c>
-    </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A108">
+      <c r="R107" s="3"/>
+      <c r="S107" s="3"/>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A108" s="3">
         <v>19875133</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="F108" t="s">
+      <c r="F108" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="G108">
+      <c r="G108" s="3">
         <v>2010</v>
       </c>
-      <c r="H108" t="s">
+      <c r="H108" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="K108" t="s">
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="L108" t="s">
+      <c r="L108" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O108" t="s">
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q108">
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3">
         <v>2010</v>
       </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A109">
+      <c r="R108" s="3"/>
+      <c r="S108" s="3"/>
+    </row>
+    <row r="109" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="3">
         <v>15224704</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F109" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="G109">
+      <c r="G109" s="3">
         <v>2004</v>
       </c>
-      <c r="H109" t="s">
+      <c r="H109" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="K109" t="s">
+      <c r="K109" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="L109" t="s">
+      <c r="L109" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O109" t="s">
+      <c r="O109" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q109">
+      <c r="Q109" s="3">
         <v>2004</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A110">
+    <row r="110" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="3">
         <v>22342396</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F110" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="G110">
+      <c r="G110" s="3">
         <v>2012</v>
       </c>
-      <c r="H110" t="s">
+      <c r="H110" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="K110" t="s">
+      <c r="K110" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="L110" t="s">
+      <c r="L110" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O110" t="s">
+      <c r="O110" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q110">
+      <c r="Q110" s="3">
         <v>2012</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A111">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A111" s="3">
         <v>21777229</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F111" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="G111">
+      <c r="G111" s="3">
         <v>2011</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H111" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="K111" t="s">
+      <c r="I111" s="3"/>
+      <c r="J111" s="3"/>
+      <c r="K111" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="L111" t="s">
+      <c r="L111" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O111" t="s">
+      <c r="M111" s="3"/>
+      <c r="N111" s="3"/>
+      <c r="O111" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q111">
+      <c r="P111" s="3"/>
+      <c r="Q111" s="3">
         <v>2011</v>
       </c>
-    </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A112">
+      <c r="R111" s="3"/>
+      <c r="S111" s="3"/>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A112" s="3">
         <v>20578537</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F112" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="G112">
+      <c r="G112" s="3">
         <v>2010</v>
       </c>
-      <c r="H112" t="s">
+      <c r="H112" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="L112" t="s">
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O112" t="s">
+      <c r="M112" s="3"/>
+      <c r="N112" s="3"/>
+      <c r="O112" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q112">
+      <c r="P112" s="3"/>
+      <c r="Q112" s="3">
         <v>2010</v>
       </c>
-    </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A113">
+      <c r="R112" s="3"/>
+      <c r="S112" s="3"/>
+    </row>
+    <row r="113" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="3">
         <v>16621618</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F113" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="G113">
+      <c r="G113" s="3">
         <v>2006</v>
       </c>
-      <c r="H113" t="s">
+      <c r="H113" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="K113" t="s">
+      <c r="K113" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="L113" t="s">
+      <c r="L113" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O113" t="s">
+      <c r="O113" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q113">
+      <c r="Q113" s="3">
         <v>2006</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A114">
+    <row r="114" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="3">
         <v>20739792</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="F114" t="s">
+      <c r="F114" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="G114">
+      <c r="G114" s="3">
         <v>2010</v>
       </c>
-      <c r="H114" t="s">
+      <c r="H114" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="K114" t="s">
+      <c r="K114" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="L114" t="s">
+      <c r="L114" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="O114" t="s">
+      <c r="O114" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="Q114">
+      <c r="Q114" s="3">
         <v>2010</v>
       </c>
     </row>

</xml_diff>